<commit_message>
learning writing cells in excel  from python
</commit_message>
<xml_diff>
--- a/in.xlsx
+++ b/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A11540D-CF38-0941-866D-1A0167C6B6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD8719E-4AAA-D34B-B09B-5C465595DB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{A43EAADA-B035-4E4C-9BF8-FFFB0A7B6414}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,10 +453,7 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
-        <f>SUM(B2,B4,B5,B12,B14,B17,B21,B25,B26,B30,B35,B32)</f>
-        <v>39464</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">

</xml_diff>